<commit_message>
Lagt til switcher i budsjettet
</commit_message>
<xml_diff>
--- a/dokumentasjon/budsjett.xlsx
+++ b/dokumentasjon/budsjett.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="31">
   <si>
     <t>Beskrivelse</t>
   </si>
@@ -63,6 +63,12 @@
   </si>
   <si>
     <t>HP OfficeJet 9720e printer</t>
+  </si>
+  <si>
+    <t>Switch</t>
+  </si>
+  <si>
+    <t>Multilayer switch</t>
   </si>
   <si>
     <t>Delsum; maskinvare</t>
@@ -487,14 +493,14 @@
         <v>10</v>
       </c>
       <c r="E5" s="4">
-        <v>2.0</v>
-      </c>
-      <c r="F5" s="3">
-        <v>100.0</v>
+        <v>4.0</v>
+      </c>
+      <c r="F5" s="5">
+        <v>10000.0</v>
       </c>
       <c r="G5" s="3">
-        <f>SUM(E5*F5)</f>
-        <v>200</v>
+        <f>sum(E5*F5)</f>
+        <v>40000</v>
       </c>
     </row>
     <row r="6">
@@ -506,7 +512,8 @@
       <c r="E6" s="10"/>
       <c r="F6" s="11"/>
       <c r="G6" s="12">
-        <v>200.0</v>
+        <f>sum(G5)</f>
+        <v>40000</v>
       </c>
     </row>
     <row r="7">
@@ -559,7 +566,7 @@
         <v>13369.0</v>
       </c>
       <c r="G13" s="3">
-        <f t="shared" ref="G13:G14" si="1">SUM(E13*F13)</f>
+        <f t="shared" ref="G13:G16" si="1">SUM(E13*F13)</f>
         <v>26738</v>
       </c>
     </row>
@@ -580,225 +587,257 @@
       </c>
     </row>
     <row r="15">
-      <c r="C15" s="10"/>
-      <c r="D15" s="8" t="s">
+      <c r="C15" s="2"/>
+      <c r="D15" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="E15" s="10"/>
-      <c r="F15" s="11"/>
-      <c r="G15" s="9">
-        <f>SUM(G10:G14)</f>
-        <v>126074</v>
+      <c r="E15" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="F15" s="14">
+        <v>951.0</v>
+      </c>
+      <c r="G15" s="3">
+        <f t="shared" si="1"/>
+        <v>2853</v>
       </c>
     </row>
     <row r="16">
       <c r="C16" s="2"/>
-      <c r="F16" s="6"/>
-      <c r="G16" s="3"/>
+      <c r="D16" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="E16" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="F16" s="14">
+        <v>2544.0</v>
+      </c>
+      <c r="G16" s="3">
+        <f t="shared" si="1"/>
+        <v>2544</v>
+      </c>
     </row>
     <row r="17">
-      <c r="C17" s="2"/>
-      <c r="D17" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E17" s="4">
-        <v>13.0</v>
-      </c>
-      <c r="F17" s="14">
-        <v>300.0</v>
-      </c>
-      <c r="G17" s="3">
-        <f>SUM(E17*F17)</f>
-        <v>3900</v>
+      <c r="C17" s="10"/>
+      <c r="D17" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="E17" s="10"/>
+      <c r="F17" s="11"/>
+      <c r="G17" s="9">
+        <f>SUM(G10:G16)</f>
+        <v>131471</v>
       </c>
     </row>
     <row r="18">
       <c r="C18" s="2"/>
-      <c r="D18" s="1" t="s">
-        <v>18</v>
-      </c>
       <c r="F18" s="6"/>
-      <c r="G18" s="3">
-        <f>SUM(G17)</f>
-        <v>3900</v>
-      </c>
+      <c r="G18" s="3"/>
     </row>
     <row r="19">
       <c r="C19" s="2"/>
-      <c r="F19" s="6"/>
-      <c r="G19" s="3"/>
+      <c r="D19" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E19" s="4">
+        <v>13.0</v>
+      </c>
+      <c r="F19" s="14">
+        <v>300.0</v>
+      </c>
+      <c r="G19" s="3">
+        <f>SUM(E19*F19)</f>
+        <v>3900</v>
+      </c>
     </row>
     <row r="20">
       <c r="C20" s="2"/>
       <c r="D20" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E20" s="4">
-        <v>1.0</v>
-      </c>
-      <c r="F20" s="14">
-        <v>15000.0</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="F20" s="6"/>
       <c r="G20" s="3">
-        <f>SUM(E20*F20)</f>
-        <v>15000</v>
+        <f>SUM(G19)</f>
+        <v>3900</v>
       </c>
     </row>
     <row r="21">
       <c r="C21" s="2"/>
-      <c r="D21" s="1" t="s">
-        <v>20</v>
-      </c>
       <c r="F21" s="6"/>
-      <c r="G21" s="3">
-        <f>sum(G20)</f>
-        <v>15000</v>
-      </c>
+      <c r="G21" s="3"/>
     </row>
     <row r="22">
       <c r="C22" s="2"/>
-      <c r="F22" s="6"/>
-      <c r="G22" s="3"/>
+      <c r="D22" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E22" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="F22" s="14">
+        <v>15000.0</v>
+      </c>
+      <c r="G22" s="3">
+        <f>SUM(E22*F22)</f>
+        <v>15000</v>
+      </c>
     </row>
     <row r="23">
       <c r="C23" s="2"/>
       <c r="D23" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F23" s="6"/>
-      <c r="G23" s="3"/>
+      <c r="G23" s="3">
+        <f>sum(G22)</f>
+        <v>15000</v>
+      </c>
     </row>
     <row r="24">
       <c r="C24" s="2"/>
-      <c r="D24" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="E24" s="4">
-        <v>11.0</v>
-      </c>
-      <c r="F24" s="14">
-        <v>2000.0</v>
-      </c>
-      <c r="G24" s="3">
-        <f t="shared" ref="G24:G25" si="2">sum(E24*F24)</f>
-        <v>22000</v>
-      </c>
+      <c r="F24" s="6"/>
+      <c r="G24" s="3"/>
     </row>
     <row r="25">
       <c r="C25" s="2"/>
-      <c r="D25" s="4" t="s">
+      <c r="D25" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E25" s="4">
+      <c r="F25" s="6"/>
+      <c r="G25" s="3"/>
+    </row>
+    <row r="26">
+      <c r="C26" s="2"/>
+      <c r="D26" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E26" s="4">
+        <v>11.0</v>
+      </c>
+      <c r="F26" s="14">
+        <v>2000.0</v>
+      </c>
+      <c r="G26" s="3">
+        <f t="shared" ref="G26:G27" si="2">sum(E26*F26)</f>
+        <v>22000</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="C27" s="2"/>
+      <c r="D27" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E27" s="4">
         <v>2.0</v>
       </c>
-      <c r="F25" s="14">
+      <c r="F27" s="14">
         <v>5000.0</v>
       </c>
-      <c r="G25" s="3">
+      <c r="G27" s="3">
         <f t="shared" si="2"/>
         <v>10000</v>
       </c>
-    </row>
-    <row r="26">
-      <c r="C26" s="2"/>
-      <c r="D26" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="F26" s="6"/>
-      <c r="G26" s="3">
-        <f>sum(G24:G25)</f>
-        <v>32000</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="C27" s="2"/>
-      <c r="F27" s="6"/>
-      <c r="G27" s="3"/>
     </row>
     <row r="28">
       <c r="C28" s="2"/>
       <c r="D28" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F28" s="6"/>
-      <c r="G28" s="3"/>
+      <c r="G28" s="3">
+        <f>sum(G26:G27)</f>
+        <v>32000</v>
+      </c>
     </row>
     <row r="29">
       <c r="C29" s="2"/>
-      <c r="D29" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="E29" s="4">
-        <v>12.0</v>
-      </c>
-      <c r="F29" s="14">
-        <v>699.0</v>
-      </c>
-      <c r="G29" s="3">
-        <f>sum(E29*F29)</f>
-        <v>8388</v>
-      </c>
+      <c r="F29" s="6"/>
+      <c r="G29" s="3"/>
     </row>
     <row r="30">
       <c r="C30" s="2"/>
-      <c r="D30" s="4" t="s">
+      <c r="D30" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="E30" s="4">
-        <v>1.0</v>
-      </c>
-      <c r="F30" s="15">
-        <v>0.05</v>
-      </c>
-      <c r="G30" s="5">
-        <v>10000.0</v>
-      </c>
+      <c r="F30" s="6"/>
+      <c r="G30" s="3"/>
     </row>
     <row r="31">
       <c r="C31" s="2"/>
-      <c r="F31" s="6"/>
-      <c r="G31" s="3"/>
+      <c r="D31" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E31" s="4">
+        <v>12.0</v>
+      </c>
+      <c r="F31" s="14">
+        <v>699.0</v>
+      </c>
+      <c r="G31" s="3">
+        <f>sum(E31*F31)</f>
+        <v>8388</v>
+      </c>
     </row>
     <row r="32">
-      <c r="C32" s="10"/>
-      <c r="D32" s="8" t="s">
+      <c r="C32" s="2"/>
+      <c r="D32" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E32" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="F32" s="15">
+        <v>0.05</v>
+      </c>
+      <c r="G32" s="5">
+        <v>10000.0</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="C33" s="2"/>
+      <c r="F33" s="6"/>
+      <c r="G33" s="3"/>
+    </row>
+    <row r="34">
+      <c r="C34" s="10"/>
+      <c r="D34" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="E32" s="10"/>
-      <c r="F32" s="11"/>
-      <c r="G32" s="9">
-        <f>sum(G6+G15+G18+G21+G26+G29+G30)</f>
-        <v>195562</v>
-      </c>
-    </row>
-    <row r="33">
-      <c r="C33" s="10"/>
-      <c r="D33" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="E33" s="10"/>
-      <c r="F33" s="11"/>
-      <c r="G33" s="9">
-        <f>sum(B5-G32)</f>
-        <v>104438</v>
+      <c r="E34" s="10"/>
+      <c r="F34" s="11"/>
+      <c r="G34" s="9">
+        <f>sum(G6+G17+G20+G23+G28+G31+G32)</f>
+        <v>240759</v>
       </c>
     </row>
     <row r="35">
-      <c r="F35" s="6"/>
-      <c r="G35" s="3"/>
-    </row>
-    <row r="36">
-      <c r="F36" s="3"/>
-      <c r="G36" s="3"/>
+      <c r="C35" s="10"/>
+      <c r="D35" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="E35" s="10"/>
+      <c r="F35" s="11"/>
+      <c r="G35" s="9">
+        <f>sum(B5-G34)</f>
+        <v>59241</v>
+      </c>
     </row>
     <row r="37">
-      <c r="F37" s="3"/>
+      <c r="F37" s="6"/>
       <c r="G37" s="3"/>
     </row>
     <row r="38">
       <c r="F38" s="3"/>
       <c r="G38" s="3"/>
+    </row>
+    <row r="39">
+      <c r="F39" s="3"/>
+      <c r="G39" s="3"/>
+    </row>
+    <row r="40">
+      <c r="F40" s="3"/>
+      <c r="G40" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="26">
@@ -833,7 +872,9 @@
     <hyperlink r:id="rId1" ref="D10"/>
     <hyperlink r:id="rId2" ref="D13"/>
     <hyperlink r:id="rId3" ref="D14"/>
+    <hyperlink r:id="rId4" ref="D15"/>
+    <hyperlink r:id="rId5" ref="D16"/>
   </hyperlinks>
-  <drawing r:id="rId4"/>
+  <drawing r:id="rId6"/>
 </worksheet>
 </file>
</xml_diff>